<commit_message>
added error flag for handled exception to TestNG method
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
+++ b/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="26" activeTab="29"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -3776,11 +3776,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4834,7 +4834,7 @@
       </c>
       <c r="E27" s="127"/>
       <c r="F27" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G27" s="129" t="s">
         <v>31</v>
@@ -13140,11 +13140,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19006,21 +19006,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19043,6 +19043,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -19057,12 +19065,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added CartTotal(Sum) change for SAPOrderRelated
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
+++ b/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73F7609-F9DD-4AEB-9F6A-A2EEEB401CD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07600250-A31D-457B-ABDB-DBF2428F8B13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="29" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -3867,11 +3867,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F74" sqref="F74"/>
+      <selection pane="bottomRight" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -13316,13 +13316,13 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -13337,11 +13337,11 @@
     <col min="8" max="8" width="8.7265625" style="86" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.7265625" style="86" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.26953125" style="86" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" style="86" customWidth="1"/>
     <col min="12" max="16384" width="9.1796875" style="86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="82" t="s">
         <v>34</v>
       </c>
@@ -13372,8 +13372,11 @@
       <c r="J1" s="82" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="86" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="87">
         <v>26</v>
       </c>
@@ -13405,7 +13408,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="87">
         <v>27</v>
       </c>
@@ -13437,7 +13440,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="29">
+    <row r="4" spans="1:11" ht="29">
       <c r="A4" s="87">
         <v>28</v>
       </c>
@@ -13469,7 +13472,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="87">
         <v>29</v>
       </c>
@@ -13501,7 +13504,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="87">
         <v>30</v>
       </c>
@@ -13533,7 +13536,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="87">
         <v>31</v>
       </c>
@@ -13565,7 +13568,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="87">
         <v>35</v>
       </c>
@@ -13597,7 +13600,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="87">
         <v>36</v>
       </c>
@@ -13629,7 +13632,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="86">
         <v>39</v>
       </c>
@@ -13661,7 +13664,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="86">
         <v>40</v>
       </c>
@@ -13693,7 +13696,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="86">
         <v>41</v>
       </c>
@@ -13725,7 +13728,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="81">
         <v>53</v>
       </c>
@@ -13757,7 +13760,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="57">
         <v>54</v>
       </c>
@@ -13789,7 +13792,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="89">
         <v>55</v>
       </c>
@@ -13821,7 +13824,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="89">
         <v>56</v>
       </c>
@@ -14793,10 +14796,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -14806,7 +14809,7 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="104" t="s">
         <v>34</v>
       </c>
@@ -14816,11 +14819,8 @@
       <c r="C1" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="105">
         <v>57</v>
       </c>
@@ -14831,7 +14831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" s="105">
         <v>58</v>
       </c>
@@ -14842,7 +14842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4" s="105">
         <v>59</v>
       </c>
@@ -14853,7 +14853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="115" customFormat="1">
+    <row r="5" spans="1:3" s="115" customFormat="1">
       <c r="A5" s="109">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Fixed Account creation negative scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
+++ b/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523E3243-9B27-4B70-BDF7-4CFC39E98D74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5422F55-1C19-434C-900F-4559F1439ECD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2839" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2713" uniqueCount="671">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2153,21 +2153,6 @@
   </si>
   <si>
     <t>fake388856143421153@automationjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake388856143421153@automatiVATjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake388856143421153@automatiIDjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake388856143421153@automatiwithjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake388856143421153@automatiwithoutjdg.co.za</t>
-  </si>
-  <si>
-    <t>fake388856143421153@automatiMagentojdg.co.za</t>
   </si>
 </sst>
 </file>
@@ -2357,7 +2342,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2706,6 +2691,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3942,11 +3930,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -4039,7 +4027,7 @@
         <v>503</v>
       </c>
       <c r="F2" s="127" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="129" t="s">
         <v>108</v>
@@ -4475,7 +4463,7 @@
         <v>196</v>
       </c>
       <c r="F13" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G13" s="129" t="s">
         <v>86</v>
@@ -7668,12 +7656,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H2" sqref="H2"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -16133,10 +16121,10 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -16551,8 +16539,8 @@
       <c r="E7" s="117" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="118" t="s">
-        <v>126</v>
+      <c r="F7" s="145" t="s">
+        <v>669</v>
       </c>
       <c r="G7" s="121" t="s">
         <v>116</v>
@@ -17145,8 +17133,11 @@
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{07E0AD4C-BB5A-49D2-8211-F59E9B02439D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -19099,24 +19090,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19265,32 +19238,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19307,4 +19273,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added data sheet TA279
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
+++ b/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EE2D4C-40DC-4572-B245-C1939836CF61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EC373D9-006C-4ADE-9A93-012CC829BFE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="16" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parrallel_ic_Login++" sheetId="77" r:id="rId1"/>
@@ -65,6 +65,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IC!$A$1:$Q$71</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -3852,7 +3853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06053B8-6DF3-44FB-9BCF-EBFA5CEA1EB4}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -4049,10 +4050,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="61" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="60" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0800-000000000000}">
@@ -4201,10 +4202,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="59" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0900-000000000000}">
@@ -4328,10 +4329,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="57" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="56" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0A00-000000000000}">
@@ -4584,10 +4585,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="55" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="54" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3" xr:uid="{00000000-0002-0000-0B00-000000000000}">
@@ -4679,10 +4680,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="53" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="52" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4736,10 +4737,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="51" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="50" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5469,22 +5470,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="49" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="48" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="45" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="44" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10" xr:uid="{00000000-0002-0000-0F00-000000000000}">
@@ -6147,22 +6148,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="43" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="42" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="40" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="39" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="38" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-1000-000000000000}">
@@ -6622,10 +6623,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1100-000000000000}">
@@ -6641,10 +6642,10 @@
   <dimension ref="A1:Q72"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G72" sqref="G72"/>
+      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9327,7 +9328,7 @@
     <cfRule type="duplicateValues" dxfId="79" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -9736,8 +9737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10174,7 +10175,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10407,7 +10408,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1400-000000000000}">
@@ -11318,16 +11319,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="33" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="32" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B33">
-    <cfRule type="duplicateValues" dxfId="31" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A33">
-    <cfRule type="duplicateValues" dxfId="30" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
@@ -11499,16 +11500,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="29" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="28" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B12">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12">
-    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12145,7 +12146,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12375,7 +12376,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13019,19 +13020,19 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B33:B35">
-    <cfRule type="duplicateValues" dxfId="23" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13132,10 +13133,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14072,13 +14073,13 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="18" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G13" xr:uid="{00000000-0002-0000-1D00-000000000000}">
@@ -14755,13 +14756,13 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="15" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A11">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
@@ -15131,10 +15132,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -15961,22 +15962,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B21">
-    <cfRule type="duplicateValues" dxfId="8" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A21">
-    <cfRule type="duplicateValues" dxfId="7" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-2A00-000000000000}">
@@ -16982,22 +16983,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B30">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A30">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B26">
-    <cfRule type="duplicateValues" dxfId="2" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A26">
-    <cfRule type="duplicateValues" dxfId="1" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11" xr:uid="{00000000-0002-0000-2B00-000000000000}">
@@ -17717,10 +17718,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -18689,22 +18690,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="72" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="71" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="70" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="69" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="68" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="67" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -18803,7 +18804,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18863,10 +18864,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19023,10 +19024,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="63" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="62" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0700-000000000000}">
@@ -19041,6 +19042,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19189,25 +19208,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19224,29 +19250,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding endtoend _tz changes
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
+++ b/src/test/resources/data/jdgroupUPDATEFINAL.xlsx
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2702" uniqueCount="693">
   <si>
     <t>testSuitID</t>
   </si>
@@ -1911,9 +1911,6 @@
     <t>icEmailWishlistverification</t>
   </si>
   <si>
-    <t>Invalid login creditials_No Username</t>
-  </si>
-  <si>
     <t>Samsung Toner D105L#Bluetooth Music Receiver</t>
   </si>
   <si>
@@ -2218,6 +2215,9 @@
   </si>
   <si>
     <t>Access#3</t>
+  </si>
+  <si>
+    <t>Invalid_login_creditials_No_Username</t>
   </si>
 </sst>
 </file>
@@ -2795,37 +2795,7 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="95">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="92">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4046,13 +4016,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S72"/>
+  <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2:F72"/>
+      <selection pane="bottomRight" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4129,10 +4099,10 @@
         <v>301</v>
       </c>
       <c r="R1" s="148" t="s">
+        <v>681</v>
+      </c>
+      <c r="S1" s="148" t="s">
         <v>682</v>
-      </c>
-      <c r="S1" s="148" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="30">
@@ -4152,7 +4122,7 @@
         <v>502</v>
       </c>
       <c r="F2" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="129" t="s">
         <v>108</v>
@@ -4192,7 +4162,7 @@
         <v>502</v>
       </c>
       <c r="F3" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3" s="129" t="s">
         <v>108</v>
@@ -4233,7 +4203,7 @@
         <v>502</v>
       </c>
       <c r="F4" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="129" t="s">
         <v>108</v>
@@ -4272,7 +4242,7 @@
         <v>502</v>
       </c>
       <c r="F5" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" s="129" t="s">
         <v>108</v>
@@ -4313,7 +4283,7 @@
         <v>502</v>
       </c>
       <c r="F6" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" s="129" t="s">
         <v>108</v>
@@ -4354,7 +4324,7 @@
         <v>136</v>
       </c>
       <c r="F7" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G7" s="129" t="s">
         <v>86</v>
@@ -4393,7 +4363,7 @@
         <v>502</v>
       </c>
       <c r="F8" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8" s="129" t="s">
         <v>86</v>
@@ -4432,7 +4402,7 @@
         <v>502</v>
       </c>
       <c r="F9" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G9" s="129" t="s">
         <v>86</v>
@@ -4469,7 +4439,7 @@
         <v>196</v>
       </c>
       <c r="F10" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10" s="129" t="s">
         <v>86</v>
@@ -4508,7 +4478,7 @@
         <v>196</v>
       </c>
       <c r="F11" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G11" s="129" t="s">
         <v>86</v>
@@ -4547,7 +4517,7 @@
         <v>196</v>
       </c>
       <c r="F12" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G12" s="129" t="s">
         <v>86</v>
@@ -4586,7 +4556,7 @@
         <v>196</v>
       </c>
       <c r="F13" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G13" s="129" t="s">
         <v>86</v>
@@ -4625,7 +4595,7 @@
         <v>196</v>
       </c>
       <c r="F14" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G14" s="129" t="s">
         <v>86</v>
@@ -4664,7 +4634,7 @@
         <v>196</v>
       </c>
       <c r="F15" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15" s="129" t="s">
         <v>86</v>
@@ -4703,7 +4673,7 @@
         <v>196</v>
       </c>
       <c r="F16" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G16" s="129" t="s">
         <v>154</v>
@@ -4746,7 +4716,7 @@
         <v>196</v>
       </c>
       <c r="F17" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G17" s="129" t="s">
         <v>154</v>
@@ -4789,7 +4759,7 @@
         <v>196</v>
       </c>
       <c r="F18" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G18" s="129" t="s">
         <v>154</v>
@@ -4832,7 +4802,7 @@
         <v>196</v>
       </c>
       <c r="F19" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G19" s="129" t="s">
         <v>154</v>
@@ -4875,7 +4845,7 @@
         <v>196</v>
       </c>
       <c r="F20" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G20" s="129" t="s">
         <v>154</v>
@@ -4918,7 +4888,7 @@
         <v>196</v>
       </c>
       <c r="F21" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G21" s="129" t="s">
         <v>154</v>
@@ -4959,7 +4929,7 @@
       </c>
       <c r="E22" s="127"/>
       <c r="F22" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G22" s="129" t="s">
         <v>108</v>
@@ -4989,7 +4959,7 @@
       </c>
       <c r="E23" s="127"/>
       <c r="F23" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G23" s="129" t="s">
         <v>108</v>
@@ -5019,7 +4989,7 @@
       </c>
       <c r="E24" s="127"/>
       <c r="F24" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G24" s="129" t="s">
         <v>108</v>
@@ -5049,7 +5019,7 @@
       </c>
       <c r="E25" s="127"/>
       <c r="F25" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G25" s="129" t="s">
         <v>108</v>
@@ -5079,7 +5049,7 @@
       </c>
       <c r="E26" s="127"/>
       <c r="F26" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G26" s="129" t="s">
         <v>108</v>
@@ -5109,7 +5079,7 @@
       </c>
       <c r="E27" s="127"/>
       <c r="F27" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G27" s="129" t="s">
         <v>31</v>
@@ -5155,7 +5125,7 @@
       </c>
       <c r="E28" s="128"/>
       <c r="F28" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G28" s="129" t="s">
         <v>31</v>
@@ -5201,7 +5171,7 @@
       </c>
       <c r="E29" s="128"/>
       <c r="F29" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G29" s="129" t="s">
         <v>31</v>
@@ -5237,17 +5207,17 @@
         <v>29</v>
       </c>
       <c r="B30" s="127" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C30" s="71" t="s">
         <v>261</v>
       </c>
       <c r="D30" s="127" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E30" s="128"/>
       <c r="F30" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G30" s="129" t="s">
         <v>31</v>
@@ -5283,17 +5253,17 @@
         <v>30</v>
       </c>
       <c r="B31" s="127" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C31" s="71" t="s">
         <v>261</v>
       </c>
       <c r="D31" s="127" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E31" s="128"/>
       <c r="F31" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G31" s="129" t="s">
         <v>31</v>
@@ -5305,7 +5275,7 @@
         <v>32</v>
       </c>
       <c r="J31" s="130" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K31" s="130" t="s">
         <v>268</v>
@@ -5327,7 +5297,7 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="143">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="B32" s="127" t="s">
         <v>514</v>
@@ -5340,50 +5310,60 @@
       </c>
       <c r="E32" s="128"/>
       <c r="F32" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G32" s="129" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="129" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="130" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="130" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="129" t="s">
+        <v>268</v>
+      </c>
+      <c r="L32" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="H32" s="129" t="s">
+      <c r="M32" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="I32" s="130" t="s">
+      <c r="N32" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="J32" s="130" t="s">
-        <v>298</v>
-      </c>
-      <c r="K32" s="130" t="s">
+      <c r="O32" s="130" t="s">
         <v>195</v>
       </c>
-      <c r="L32" s="130" t="s">
+      <c r="P32" s="130" t="s">
         <v>210</v>
       </c>
-      <c r="M32" s="129"/>
-      <c r="N32" s="130"/>
-      <c r="O32" s="127"/>
-      <c r="P32" s="127"/>
     </row>
     <row r="33" spans="1:19">
-      <c r="A33" s="143">
-        <v>31</v>
+      <c r="A33" s="61">
+        <v>32</v>
       </c>
       <c r="B33" s="127" t="s">
-        <v>514</v>
-      </c>
-      <c r="C33" s="71" t="s">
-        <v>270</v>
+        <v>546</v>
+      </c>
+      <c r="C33" s="70" t="s">
+        <v>261</v>
       </c>
       <c r="D33" s="127" t="s">
-        <v>514</v>
-      </c>
-      <c r="E33" s="128"/>
+        <v>546</v>
+      </c>
+      <c r="E33" s="128" t="s">
+        <v>196</v>
+      </c>
       <c r="F33" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="129" t="s">
-        <v>31</v>
+        <v>9</v>
+      </c>
+      <c r="G33" s="130" t="s">
+        <v>155</v>
       </c>
       <c r="H33" s="129" t="s">
         <v>57</v>
@@ -5395,198 +5375,190 @@
         <v>33</v>
       </c>
       <c r="K33" s="129" t="s">
-        <v>268</v>
+        <v>86</v>
       </c>
       <c r="L33" s="129" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M33" s="129" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="N33" s="130" t="s">
-        <v>109</v>
-      </c>
-      <c r="O33" s="130" t="s">
         <v>195</v>
       </c>
-      <c r="P33" s="130" t="s">
-        <v>210</v>
-      </c>
+      <c r="O33" s="127"/>
+      <c r="P33" s="127"/>
     </row>
     <row r="34" spans="1:19">
       <c r="A34" s="61">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="127" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C34" s="70" t="s">
         <v>261</v>
       </c>
       <c r="D34" s="127" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E34" s="128" t="s">
         <v>196</v>
       </c>
       <c r="F34" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G34" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="H34" s="130" t="s">
         <v>155</v>
       </c>
-      <c r="H34" s="129" t="s">
-        <v>57</v>
-      </c>
-      <c r="I34" s="130" t="s">
+      <c r="I34" s="127" t="s">
+        <v>198</v>
+      </c>
+      <c r="J34" s="130" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="130" t="s">
+      <c r="K34" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="K34" s="129" t="s">
+      <c r="L34" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="L34" s="129" t="s">
+      <c r="M34" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="M34" s="129" t="s">
+      <c r="N34" s="129" t="s">
         <v>109</v>
       </c>
-      <c r="N34" s="130" t="s">
+      <c r="O34" s="130" t="s">
         <v>195</v>
       </c>
-      <c r="O34" s="127"/>
       <c r="P34" s="127"/>
+      <c r="Q34" s="127"/>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" s="61">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="127" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C35" s="70" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="D35" s="127" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E35" s="128" t="s">
         <v>196</v>
       </c>
       <c r="F35" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G35" s="130" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H35" s="130" t="s">
-        <v>155</v>
-      </c>
-      <c r="I35" s="127" t="s">
-        <v>198</v>
+        <v>32</v>
+      </c>
+      <c r="I35" s="130" t="s">
+        <v>33</v>
       </c>
       <c r="J35" s="130" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="K35" s="130" t="s">
-        <v>33</v>
-      </c>
-      <c r="L35" s="129" t="s">
-        <v>86</v>
-      </c>
-      <c r="M35" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="N35" s="129" t="s">
+      <c r="L35" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="O35" s="130" t="s">
+      <c r="M35" s="130" t="s">
         <v>195</v>
       </c>
+      <c r="N35" s="127"/>
+      <c r="O35" s="127"/>
       <c r="P35" s="127"/>
-      <c r="Q35" s="127"/>
     </row>
     <row r="36" spans="1:19">
       <c r="A36" s="61">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="127" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C36" s="70" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D36" s="127" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E36" s="128" t="s">
         <v>196</v>
       </c>
       <c r="F36" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="130" t="s">
-        <v>155</v>
-      </c>
-      <c r="H36" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="129" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" s="129" t="s">
+        <v>197</v>
+      </c>
+      <c r="I36" s="129" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="130" t="s">
         <v>32</v>
       </c>
-      <c r="I36" s="130" t="s">
+      <c r="K36" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="J36" s="130" t="s">
-        <v>86</v>
-      </c>
-      <c r="K36" s="130" t="s">
-        <v>88</v>
-      </c>
-      <c r="L36" s="130" t="s">
-        <v>109</v>
-      </c>
-      <c r="M36" s="130" t="s">
-        <v>195</v>
-      </c>
+      <c r="L36" s="127"/>
+      <c r="M36" s="127"/>
       <c r="N36" s="127"/>
       <c r="O36" s="127"/>
       <c r="P36" s="127"/>
     </row>
     <row r="37" spans="1:19">
       <c r="A37" s="61">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="127" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C37" s="70" t="s">
         <v>272</v>
       </c>
       <c r="D37" s="127" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E37" s="128" t="s">
         <v>196</v>
       </c>
       <c r="F37" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="129" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="H37" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="129" t="s">
+      <c r="I37" s="129" t="s">
         <v>197</v>
       </c>
-      <c r="I37" s="129" t="s">
-        <v>57</v>
-      </c>
-      <c r="J37" s="130" t="s">
+      <c r="J37" s="127" t="s">
+        <v>198</v>
+      </c>
+      <c r="K37" s="130" t="s">
         <v>32</v>
       </c>
-      <c r="K37" s="130" t="s">
+      <c r="L37" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="L37" s="127"/>
       <c r="M37" s="127"/>
       <c r="N37" s="127"/>
       <c r="O37" s="127"/>
@@ -5594,41 +5566,33 @@
     </row>
     <row r="38" spans="1:19">
       <c r="A38" s="61">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="127" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C38" s="70" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D38" s="127" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E38" s="128" t="s">
         <v>196</v>
       </c>
       <c r="F38" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="130" t="s">
-        <v>154</v>
-      </c>
-      <c r="H38" s="129" t="s">
-        <v>31</v>
-      </c>
-      <c r="I38" s="129" t="s">
-        <v>197</v>
-      </c>
-      <c r="J38" s="127" t="s">
-        <v>198</v>
-      </c>
-      <c r="K38" s="130" t="s">
-        <v>32</v>
-      </c>
-      <c r="L38" s="130" t="s">
-        <v>33</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G38" s="132" t="s">
+        <v>86</v>
+      </c>
+      <c r="H38" s="132" t="s">
+        <v>275</v>
+      </c>
+      <c r="I38" s="129"/>
+      <c r="J38" s="130"/>
+      <c r="K38" s="127"/>
+      <c r="L38" s="127"/>
       <c r="M38" s="127"/>
       <c r="N38" s="127"/>
       <c r="O38" s="127"/>
@@ -5636,22 +5600,22 @@
     </row>
     <row r="39" spans="1:19">
       <c r="A39" s="61">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="127" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C39" s="70" t="s">
         <v>274</v>
       </c>
       <c r="D39" s="127" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E39" s="128" t="s">
         <v>196</v>
       </c>
       <c r="F39" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G39" s="132" t="s">
         <v>86</v>
@@ -5669,53 +5633,74 @@
       <c r="P39" s="127"/>
     </row>
     <row r="40" spans="1:19">
-      <c r="A40" s="61">
-        <v>38</v>
-      </c>
-      <c r="B40" s="127" t="s">
-        <v>540</v>
-      </c>
-      <c r="C40" s="70" t="s">
-        <v>274</v>
-      </c>
-      <c r="D40" s="127" t="s">
-        <v>540</v>
-      </c>
-      <c r="E40" s="128" t="s">
-        <v>196</v>
-      </c>
+      <c r="A40" s="145">
+        <v>39</v>
+      </c>
+      <c r="B40" s="134" t="s">
+        <v>515</v>
+      </c>
+      <c r="C40" s="70"/>
+      <c r="D40" s="134" t="s">
+        <v>515</v>
+      </c>
+      <c r="E40" s="128"/>
       <c r="F40" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G40" s="132" t="s">
+        <v>154</v>
+      </c>
+      <c r="H40" s="132" t="s">
+        <v>577</v>
+      </c>
+      <c r="I40" s="132" t="s">
+        <v>31</v>
+      </c>
+      <c r="J40" s="132" t="s">
+        <v>57</v>
+      </c>
+      <c r="K40" s="132" t="s">
+        <v>32</v>
+      </c>
+      <c r="L40" s="132" t="s">
+        <v>33</v>
+      </c>
+      <c r="M40" s="132" t="s">
         <v>86</v>
       </c>
-      <c r="H40" s="132" t="s">
-        <v>275</v>
-      </c>
-      <c r="I40" s="129"/>
-      <c r="J40" s="130"/>
-      <c r="K40" s="127"/>
-      <c r="L40" s="127"/>
-      <c r="M40" s="127"/>
-      <c r="N40" s="127"/>
-      <c r="O40" s="127"/>
-      <c r="P40" s="127"/>
+      <c r="N40" s="132" t="s">
+        <v>88</v>
+      </c>
+      <c r="O40" s="132" t="s">
+        <v>109</v>
+      </c>
+      <c r="P40" s="115" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q40" s="138" t="s">
+        <v>298</v>
+      </c>
+      <c r="R40" s="130" t="s">
+        <v>195</v>
+      </c>
+      <c r="S40" s="132" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="145">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="134" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C41" s="70"/>
       <c r="D41" s="134" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E41" s="128"/>
       <c r="F41" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G41" s="132" t="s">
         <v>154</v>
@@ -5759,18 +5744,18 @@
     </row>
     <row r="42" spans="1:19">
       <c r="A42" s="145">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="134" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C42" s="70"/>
       <c r="D42" s="134" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E42" s="128"/>
       <c r="F42" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G42" s="132" t="s">
         <v>154</v>
@@ -5813,79 +5798,53 @@
       </c>
     </row>
     <row r="43" spans="1:19">
-      <c r="A43" s="145">
-        <v>41</v>
-      </c>
-      <c r="B43" s="134" t="s">
-        <v>517</v>
+      <c r="A43" s="63">
+        <v>42</v>
+      </c>
+      <c r="B43" s="133" t="s">
+        <v>518</v>
       </c>
       <c r="C43" s="70"/>
-      <c r="D43" s="134" t="s">
-        <v>517</v>
-      </c>
-      <c r="E43" s="128"/>
+      <c r="D43" s="133" t="s">
+        <v>518</v>
+      </c>
+      <c r="E43" s="128" t="s">
+        <v>196</v>
+      </c>
       <c r="F43" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="132" t="s">
-        <v>154</v>
-      </c>
-      <c r="H43" s="132" t="s">
-        <v>577</v>
-      </c>
-      <c r="I43" s="132" t="s">
-        <v>31</v>
-      </c>
-      <c r="J43" s="132" t="s">
-        <v>57</v>
-      </c>
-      <c r="K43" s="132" t="s">
-        <v>32</v>
-      </c>
-      <c r="L43" s="132" t="s">
-        <v>33</v>
-      </c>
-      <c r="M43" s="132" t="s">
-        <v>86</v>
-      </c>
-      <c r="N43" s="132" t="s">
-        <v>88</v>
-      </c>
-      <c r="O43" s="132" t="s">
-        <v>109</v>
-      </c>
-      <c r="P43" s="115" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q43" s="138" t="s">
-        <v>298</v>
-      </c>
-      <c r="R43" s="130" t="s">
-        <v>195</v>
-      </c>
-      <c r="S43" s="132" t="s">
-        <v>210</v>
-      </c>
+      <c r="G43" s="133" t="s">
+        <v>287</v>
+      </c>
+      <c r="H43" s="133"/>
+      <c r="I43" s="133"/>
+      <c r="J43" s="133"/>
+      <c r="K43" s="133"/>
+      <c r="L43" s="133"/>
+      <c r="M43" s="133"/>
+      <c r="N43" s="133"/>
+      <c r="O43" s="133"/>
+      <c r="P43" s="133"/>
+      <c r="Q43" s="133"/>
     </row>
     <row r="44" spans="1:19">
       <c r="A44" s="63">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="133" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C44" s="70"/>
       <c r="D44" s="133" t="s">
-        <v>518</v>
-      </c>
-      <c r="E44" s="128" t="s">
-        <v>196</v>
-      </c>
+        <v>519</v>
+      </c>
+      <c r="E44" s="128"/>
       <c r="F44" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G44" s="133" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H44" s="133"/>
       <c r="I44" s="133"/>
@@ -5899,22 +5858,24 @@
       <c r="Q44" s="133"/>
     </row>
     <row r="45" spans="1:19">
-      <c r="A45" s="63">
-        <v>43</v>
+      <c r="A45" s="64">
+        <v>44</v>
       </c>
       <c r="B45" s="133" t="s">
-        <v>519</v>
+        <v>539</v>
       </c>
       <c r="C45" s="70"/>
       <c r="D45" s="133" t="s">
-        <v>519</v>
-      </c>
-      <c r="E45" s="128"/>
+        <v>283</v>
+      </c>
+      <c r="E45" s="128" t="s">
+        <v>196</v>
+      </c>
       <c r="F45" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G45" s="133" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H45" s="133"/>
       <c r="I45" s="133"/>
@@ -5928,24 +5889,24 @@
       <c r="Q45" s="133"/>
     </row>
     <row r="46" spans="1:19">
-      <c r="A46" s="64">
-        <v>44</v>
-      </c>
-      <c r="B46" s="133" t="s">
-        <v>539</v>
+      <c r="A46" s="63">
+        <v>45</v>
+      </c>
+      <c r="B46" s="136" t="s">
+        <v>520</v>
       </c>
       <c r="C46" s="70"/>
-      <c r="D46" s="133" t="s">
-        <v>283</v>
+      <c r="D46" s="136" t="s">
+        <v>284</v>
       </c>
       <c r="E46" s="128" t="s">
         <v>196</v>
       </c>
       <c r="F46" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="133" t="s">
-        <v>289</v>
+        <v>9</v>
+      </c>
+      <c r="G46" s="136" t="s">
+        <v>290</v>
       </c>
       <c r="H46" s="133"/>
       <c r="I46" s="133"/>
@@ -5959,52 +5920,66 @@
       <c r="Q46" s="133"/>
     </row>
     <row r="47" spans="1:19">
-      <c r="A47" s="63">
-        <v>45</v>
-      </c>
-      <c r="B47" s="136" t="s">
-        <v>520</v>
+      <c r="A47" s="65">
+        <v>46</v>
+      </c>
+      <c r="B47" s="134" t="s">
+        <v>521</v>
       </c>
       <c r="C47" s="70"/>
-      <c r="D47" s="136" t="s">
-        <v>284</v>
+      <c r="D47" s="134" t="s">
+        <v>521</v>
       </c>
       <c r="E47" s="128" t="s">
         <v>196</v>
       </c>
       <c r="F47" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G47" s="136" t="s">
-        <v>290</v>
-      </c>
-      <c r="H47" s="133"/>
-      <c r="I47" s="133"/>
-      <c r="J47" s="133"/>
-      <c r="K47" s="133"/>
-      <c r="L47" s="133"/>
-      <c r="M47" s="133"/>
-      <c r="N47" s="133"/>
-      <c r="O47" s="133"/>
-      <c r="P47" s="133"/>
-      <c r="Q47" s="133"/>
+        <v>9</v>
+      </c>
+      <c r="G47" s="132" t="s">
+        <v>154</v>
+      </c>
+      <c r="H47" s="132" t="s">
+        <v>291</v>
+      </c>
+      <c r="I47" s="132" t="s">
+        <v>292</v>
+      </c>
+      <c r="J47" s="132" t="s">
+        <v>293</v>
+      </c>
+      <c r="K47" s="132" t="s">
+        <v>294</v>
+      </c>
+      <c r="L47" s="132" t="s">
+        <v>295</v>
+      </c>
+      <c r="M47" s="132" t="s">
+        <v>86</v>
+      </c>
+      <c r="N47" s="132" t="s">
+        <v>285</v>
+      </c>
+      <c r="O47" s="132" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="65">
-        <v>46</v>
-      </c>
-      <c r="B48" s="134" t="s">
-        <v>521</v>
+        <v>47</v>
+      </c>
+      <c r="B48" s="137" t="s">
+        <v>419</v>
       </c>
       <c r="C48" s="70"/>
       <c r="D48" s="134" t="s">
-        <v>521</v>
+        <v>431</v>
       </c>
       <c r="E48" s="128" t="s">
-        <v>196</v>
+        <v>136</v>
       </c>
       <c r="F48" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G48" s="132" t="s">
         <v>154</v>
@@ -6024,94 +5999,73 @@
       <c r="L48" s="132" t="s">
         <v>295</v>
       </c>
-      <c r="M48" s="132" t="s">
-        <v>86</v>
-      </c>
-      <c r="N48" s="132" t="s">
-        <v>285</v>
-      </c>
-      <c r="O48" s="132" t="s">
-        <v>286</v>
-      </c>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="65">
-        <v>47</v>
+      <c r="A49" s="62">
+        <v>48</v>
       </c>
       <c r="B49" s="137" t="s">
-        <v>419</v>
+        <v>538</v>
       </c>
       <c r="C49" s="70"/>
-      <c r="D49" s="134" t="s">
-        <v>431</v>
-      </c>
-      <c r="E49" s="128" t="s">
-        <v>136</v>
-      </c>
+      <c r="D49" s="137" t="s">
+        <v>538</v>
+      </c>
+      <c r="E49" s="128"/>
       <c r="F49" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G49" s="132" t="s">
-        <v>154</v>
-      </c>
-      <c r="H49" s="132" t="s">
-        <v>291</v>
-      </c>
-      <c r="I49" s="132" t="s">
-        <v>292</v>
-      </c>
-      <c r="J49" s="132" t="s">
-        <v>293</v>
-      </c>
-      <c r="K49" s="132" t="s">
-        <v>294</v>
-      </c>
-      <c r="L49" s="132" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16">
-      <c r="A50" s="62">
-        <v>48</v>
-      </c>
-      <c r="B50" s="137" t="s">
-        <v>538</v>
-      </c>
-      <c r="C50" s="70"/>
-      <c r="D50" s="137" t="s">
-        <v>538</v>
-      </c>
-      <c r="E50" s="128"/>
+        <v>296</v>
+      </c>
+      <c r="J49" s="135"/>
+      <c r="K49" s="135"/>
+      <c r="L49" s="132"/>
+      <c r="N49" s="132"/>
+      <c r="O49" s="135"/>
+    </row>
+    <row r="50" spans="1:16" s="57" customFormat="1">
+      <c r="A50" s="66">
+        <v>49</v>
+      </c>
+      <c r="B50" s="126" t="s">
+        <v>522</v>
+      </c>
+      <c r="C50" s="69">
+        <v>215</v>
+      </c>
+      <c r="D50" s="126" t="s">
+        <v>522</v>
+      </c>
+      <c r="E50" s="128" t="s">
+        <v>502</v>
+      </c>
       <c r="F50" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" s="132" t="s">
-        <v>296</v>
-      </c>
-      <c r="J50" s="135"/>
-      <c r="K50" s="135"/>
-      <c r="L50" s="132"/>
-      <c r="N50" s="132"/>
-      <c r="O50" s="135"/>
+        <v>9</v>
+      </c>
+      <c r="G50" s="58" t="s">
+        <v>297</v>
+      </c>
+      <c r="H50" s="126"/>
     </row>
     <row r="51" spans="1:16" s="57" customFormat="1">
       <c r="A51" s="66">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" s="126" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C51" s="69">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D51" s="126" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E51" s="128" t="s">
         <v>502</v>
       </c>
       <c r="F51" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G51" s="58" t="s">
         <v>297</v>
@@ -6120,123 +6074,135 @@
     </row>
     <row r="52" spans="1:16" s="57" customFormat="1">
       <c r="A52" s="66">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="126" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C52" s="69">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D52" s="126" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E52" s="128" t="s">
         <v>502</v>
       </c>
       <c r="F52" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G52" s="58" t="s">
         <v>297</v>
       </c>
       <c r="H52" s="126"/>
     </row>
-    <row r="53" spans="1:16" s="57" customFormat="1">
-      <c r="A53" s="66">
-        <v>51</v>
-      </c>
-      <c r="B53" s="126" t="s">
-        <v>524</v>
-      </c>
-      <c r="C53" s="69">
-        <v>217</v>
-      </c>
-      <c r="D53" s="126" t="s">
-        <v>524</v>
-      </c>
-      <c r="E53" s="128" t="s">
-        <v>502</v>
+    <row r="53" spans="1:16" s="133" customFormat="1">
+      <c r="A53" s="64">
+        <v>52</v>
+      </c>
+      <c r="B53" s="133" t="s">
+        <v>537</v>
+      </c>
+      <c r="C53" s="64"/>
+      <c r="D53" s="133" t="s">
+        <v>537</v>
+      </c>
+      <c r="E53" s="133" t="s">
+        <v>136</v>
       </c>
       <c r="F53" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="58" t="s">
-        <v>297</v>
-      </c>
-      <c r="H53" s="126"/>
+        <v>9</v>
+      </c>
+      <c r="G53" s="132" t="s">
+        <v>408</v>
+      </c>
+      <c r="H53" s="132" t="s">
+        <v>409</v>
+      </c>
+      <c r="I53" s="132" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="54" spans="1:16" s="133" customFormat="1">
       <c r="A54" s="64">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54" s="133" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C54" s="64"/>
       <c r="D54" s="133" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E54" s="133" t="s">
         <v>136</v>
       </c>
       <c r="F54" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G54" s="132" t="s">
         <v>408</v>
       </c>
       <c r="H54" s="132" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" s="132" t="s">
         <v>409</v>
       </c>
-      <c r="I54" s="132" t="s">
+      <c r="J54" s="132" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="133" customFormat="1">
-      <c r="A55" s="64">
-        <v>53</v>
-      </c>
-      <c r="B55" s="133" t="s">
-        <v>536</v>
-      </c>
-      <c r="C55" s="64"/>
-      <c r="D55" s="133" t="s">
-        <v>536</v>
-      </c>
-      <c r="E55" s="133" t="s">
-        <v>136</v>
-      </c>
+    <row r="55" spans="1:16">
+      <c r="A55" s="69">
+        <v>54</v>
+      </c>
+      <c r="B55" s="67" t="s">
+        <v>615</v>
+      </c>
+      <c r="C55" s="69"/>
+      <c r="D55" s="67" t="s">
+        <v>615</v>
+      </c>
+      <c r="E55" s="57"/>
       <c r="F55" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" s="132" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" s="58" t="s">
         <v>408</v>
       </c>
-      <c r="H55" s="132" t="s">
+      <c r="H55" s="58" t="s">
+        <v>409</v>
+      </c>
+      <c r="I55" s="58" t="s">
+        <v>410</v>
+      </c>
+      <c r="J55" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="I55" s="132" t="s">
-        <v>409</v>
-      </c>
-      <c r="J55" s="132" t="s">
-        <v>410</v>
-      </c>
+      <c r="K55" s="58" t="s">
+        <v>576</v>
+      </c>
+      <c r="L55" s="57"/>
+      <c r="M55" s="57"/>
+      <c r="N55" s="57"/>
+      <c r="O55" s="57"/>
+      <c r="P55" s="127"/>
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="69">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" s="67" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C56" s="69"/>
       <c r="D56" s="67" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E56" s="57"/>
       <c r="F56" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G56" s="58" t="s">
         <v>408</v>
@@ -6250,29 +6216,26 @@
       <c r="J56" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="K56" s="58" t="s">
-        <v>576</v>
-      </c>
+      <c r="K56" s="57"/>
       <c r="L56" s="57"/>
       <c r="M56" s="57"/>
       <c r="N56" s="57"/>
       <c r="O56" s="57"/>
-      <c r="P56" s="127"/>
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="69">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" s="67" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C57" s="69"/>
       <c r="D57" s="67" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="E57" s="57"/>
       <c r="F57" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G57" s="58" t="s">
         <v>408</v>
@@ -6286,7 +6249,9 @@
       <c r="J57" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="K57" s="57"/>
+      <c r="K57" s="58" t="s">
+        <v>409</v>
+      </c>
       <c r="L57" s="57"/>
       <c r="M57" s="57"/>
       <c r="N57" s="57"/>
@@ -6294,34 +6259,32 @@
     </row>
     <row r="58" spans="1:16">
       <c r="A58" s="69">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58" s="67" t="s">
         <v>617</v>
       </c>
-      <c r="C58" s="69"/>
+      <c r="C58" s="69">
+        <v>265</v>
+      </c>
       <c r="D58" s="67" t="s">
         <v>617</v>
       </c>
-      <c r="E58" s="57"/>
+      <c r="E58" s="68" t="s">
+        <v>502</v>
+      </c>
       <c r="F58" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G58" s="58" t="s">
-        <v>408</v>
+        <v>154</v>
       </c>
       <c r="H58" s="58" t="s">
-        <v>409</v>
-      </c>
-      <c r="I58" s="58" t="s">
-        <v>410</v>
-      </c>
-      <c r="J58" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="K58" s="58" t="s">
-        <v>409</v>
-      </c>
+        <v>577</v>
+      </c>
+      <c r="I58" s="57"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="57"/>
       <c r="L58" s="57"/>
       <c r="M58" s="57"/>
       <c r="N58" s="57"/>
@@ -6329,13 +6292,13 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" s="69">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B59" s="67" t="s">
         <v>618</v>
       </c>
       <c r="C59" s="69">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D59" s="67" t="s">
         <v>618</v>
@@ -6344,15 +6307,15 @@
         <v>502</v>
       </c>
       <c r="F59" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G59" s="58" t="s">
-        <v>154</v>
+        <v>577</v>
       </c>
       <c r="H59" s="58" t="s">
-        <v>577</v>
-      </c>
-      <c r="I59" s="57"/>
+        <v>31</v>
+      </c>
+      <c r="I59" s="67"/>
       <c r="J59" s="57"/>
       <c r="K59" s="57"/>
       <c r="L59" s="57"/>
@@ -6362,13 +6325,13 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="69">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60" s="67" t="s">
         <v>619</v>
       </c>
       <c r="C60" s="69">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D60" s="67" t="s">
         <v>619</v>
@@ -6377,7 +6340,7 @@
         <v>502</v>
       </c>
       <c r="F60" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G60" s="58" t="s">
         <v>577</v>
@@ -6385,7 +6348,7 @@
       <c r="H60" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="I60" s="67"/>
+      <c r="I60" s="57"/>
       <c r="J60" s="57"/>
       <c r="K60" s="57"/>
       <c r="L60" s="57"/>
@@ -6395,13 +6358,13 @@
     </row>
     <row r="61" spans="1:16">
       <c r="A61" s="69">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" s="67" t="s">
         <v>620</v>
       </c>
       <c r="C61" s="69">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D61" s="67" t="s">
         <v>620</v>
@@ -6410,13 +6373,13 @@
         <v>502</v>
       </c>
       <c r="F61" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G61" s="58" t="s">
-        <v>577</v>
-      </c>
-      <c r="H61" s="58" t="s">
         <v>31</v>
+      </c>
+      <c r="H61" s="67" t="s">
+        <v>578</v>
       </c>
       <c r="I61" s="57"/>
       <c r="J61" s="57"/>
@@ -6428,14 +6391,12 @@
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="69">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B62" s="67" t="s">
         <v>621</v>
       </c>
-      <c r="C62" s="69">
-        <v>270</v>
-      </c>
+      <c r="C62" s="69"/>
       <c r="D62" s="67" t="s">
         <v>621</v>
       </c>
@@ -6443,13 +6404,13 @@
         <v>502</v>
       </c>
       <c r="F62" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G62" s="58" t="s">
         <v>31</v>
       </c>
       <c r="H62" s="67" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="I62" s="57"/>
       <c r="J62" s="57"/>
@@ -6461,27 +6422,27 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="69">
-        <v>61</v>
-      </c>
-      <c r="B63" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="72" t="s">
         <v>622</v>
       </c>
-      <c r="C63" s="69"/>
+      <c r="C63" s="69">
+        <v>305</v>
+      </c>
       <c r="D63" s="67" t="s">
-        <v>622</v>
+        <v>580</v>
       </c>
       <c r="E63" s="68" t="s">
-        <v>502</v>
+        <v>196</v>
       </c>
       <c r="F63" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G63" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H63" s="67" t="s">
-        <v>579</v>
-      </c>
+        <v>581</v>
+      </c>
+      <c r="H63" s="57"/>
       <c r="I63" s="57"/>
       <c r="J63" s="57"/>
       <c r="K63" s="57"/>
@@ -6492,10 +6453,10 @@
     </row>
     <row r="64" spans="1:16">
       <c r="A64" s="69">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B64" s="72" t="s">
-        <v>623</v>
+        <v>692</v>
       </c>
       <c r="C64" s="69">
         <v>305</v>
@@ -6507,7 +6468,7 @@
         <v>196</v>
       </c>
       <c r="F64" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G64" s="58" t="s">
         <v>581</v>
@@ -6521,58 +6482,55 @@
       <c r="N64" s="57"/>
       <c r="O64" s="57"/>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:12">
       <c r="A65" s="69">
-        <v>63</v>
-      </c>
-      <c r="B65" s="72" t="s">
-        <v>590</v>
+        <v>64</v>
+      </c>
+      <c r="B65" s="73" t="s">
+        <v>623</v>
       </c>
       <c r="C65" s="69">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D65" s="67" t="s">
-        <v>580</v>
+        <v>623</v>
       </c>
       <c r="E65" s="68" t="s">
         <v>196</v>
       </c>
       <c r="F65" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G65" s="58" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="H65" s="57"/>
       <c r="I65" s="57"/>
       <c r="J65" s="57"/>
       <c r="K65" s="57"/>
       <c r="L65" s="57"/>
-      <c r="M65" s="57"/>
-      <c r="N65" s="57"/>
-      <c r="O65" s="57"/>
-    </row>
-    <row r="66" spans="1:15">
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" s="69">
-        <v>64</v>
-      </c>
-      <c r="B66" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="67" t="s">
         <v>624</v>
       </c>
       <c r="C66" s="69">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D66" s="67" t="s">
         <v>624</v>
       </c>
-      <c r="E66" s="68" t="s">
+      <c r="E66" s="67" t="s">
         <v>196</v>
       </c>
       <c r="F66" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G66" s="58" t="s">
-        <v>582</v>
+        <v>9</v>
+      </c>
+      <c r="G66" s="57" t="s">
+        <v>583</v>
       </c>
       <c r="H66" s="57"/>
       <c r="I66" s="57"/>
@@ -6580,15 +6538,15 @@
       <c r="K66" s="57"/>
       <c r="L66" s="57"/>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:12">
       <c r="A67" s="69">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B67" s="67" t="s">
         <v>625</v>
       </c>
       <c r="C67" s="69">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D67" s="67" t="s">
         <v>625</v>
@@ -6597,10 +6555,10 @@
         <v>196</v>
       </c>
       <c r="F67" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G67" s="57" t="s">
-        <v>583</v>
+        <v>9</v>
+      </c>
+      <c r="G67" s="68" t="s">
+        <v>584</v>
       </c>
       <c r="H67" s="57"/>
       <c r="I67" s="57"/>
@@ -6608,15 +6566,15 @@
       <c r="K67" s="57"/>
       <c r="L67" s="57"/>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:12">
       <c r="A68" s="69">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B68" s="67" t="s">
         <v>626</v>
       </c>
       <c r="C68" s="69">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D68" s="67" t="s">
         <v>626</v>
@@ -6625,174 +6583,137 @@
         <v>196</v>
       </c>
       <c r="F68" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G68" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68" s="57" t="s">
         <v>584</v>
       </c>
-      <c r="H68" s="57"/>
+      <c r="H68" s="67" t="s">
+        <v>585</v>
+      </c>
       <c r="I68" s="57"/>
       <c r="J68" s="57"/>
       <c r="K68" s="57"/>
       <c r="L68" s="57"/>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:12">
       <c r="A69" s="69">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B69" s="67" t="s">
         <v>627</v>
       </c>
       <c r="C69" s="69">
-        <v>318</v>
-      </c>
-      <c r="D69" s="67" t="s">
+        <v>331</v>
+      </c>
+      <c r="D69" s="126" t="s">
         <v>627</v>
       </c>
       <c r="E69" s="67" t="s">
         <v>196</v>
       </c>
       <c r="F69" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G69" s="57" t="s">
-        <v>584</v>
-      </c>
-      <c r="H69" s="67" t="s">
-        <v>585</v>
-      </c>
-      <c r="I69" s="57"/>
-      <c r="J69" s="57"/>
+        <v>9</v>
+      </c>
+      <c r="G69" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H69" s="58"/>
+      <c r="I69" s="67"/>
+      <c r="J69" s="67"/>
       <c r="K69" s="57"/>
       <c r="L69" s="57"/>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:12">
       <c r="A70" s="69">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B70" s="67" t="s">
         <v>628</v>
       </c>
       <c r="C70" s="69">
-        <v>331</v>
-      </c>
-      <c r="D70" s="126" t="s">
+        <v>335</v>
+      </c>
+      <c r="D70" s="67" t="s">
         <v>628</v>
       </c>
-      <c r="E70" s="67" t="s">
-        <v>196</v>
-      </c>
+      <c r="E70" s="57"/>
       <c r="F70" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G70" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H70" s="58"/>
-      <c r="I70" s="67"/>
-      <c r="J70" s="67"/>
+      <c r="H70" s="57" t="s">
+        <v>586</v>
+      </c>
+      <c r="I70" s="57"/>
+      <c r="J70" s="57"/>
       <c r="K70" s="57"/>
       <c r="L70" s="57"/>
     </row>
-    <row r="71" spans="1:15">
-      <c r="A71" s="69">
-        <v>69</v>
+    <row r="71" spans="1:12">
+      <c r="A71" s="66">
+        <v>70</v>
       </c>
       <c r="B71" s="67" t="s">
         <v>629</v>
       </c>
       <c r="C71" s="69">
-        <v>335</v>
+        <v>265</v>
       </c>
       <c r="D71" s="67" t="s">
         <v>629</v>
       </c>
-      <c r="E71" s="57"/>
+      <c r="E71" s="68" t="s">
+        <v>587</v>
+      </c>
       <c r="F71" s="127" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G71" s="58" t="s">
+        <v>408</v>
+      </c>
+      <c r="H71" s="58" t="s">
+        <v>409</v>
+      </c>
+      <c r="I71" s="58" t="s">
+        <v>410</v>
+      </c>
+      <c r="J71" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H71" s="57" t="s">
-        <v>586</v>
-      </c>
-      <c r="I71" s="57"/>
-      <c r="J71" s="57"/>
-      <c r="K71" s="57"/>
-      <c r="L71" s="57"/>
-    </row>
-    <row r="72" spans="1:15">
-      <c r="A72" s="66">
-        <v>70</v>
-      </c>
-      <c r="B72" s="67" t="s">
-        <v>630</v>
-      </c>
-      <c r="C72" s="69">
-        <v>265</v>
-      </c>
-      <c r="D72" s="67" t="s">
-        <v>630</v>
-      </c>
-      <c r="E72" s="68" t="s">
-        <v>587</v>
-      </c>
-      <c r="F72" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="G72" s="58" t="s">
-        <v>408</v>
-      </c>
-      <c r="H72" s="58" t="s">
-        <v>409</v>
-      </c>
-      <c r="I72" s="58" t="s">
-        <v>410</v>
-      </c>
-      <c r="J72" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="K72" s="58" t="s">
+      <c r="K71" s="58" t="s">
         <v>588</v>
       </c>
-      <c r="L72" s="58" t="s">
+      <c r="L71" s="58" t="s">
         <v>589</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B54:B55">
-    <cfRule type="duplicateValues" dxfId="94" priority="14"/>
+  <conditionalFormatting sqref="B53:B54">
+    <cfRule type="duplicateValues" dxfId="91" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:B50 B1:B31 B56:B1048576">
-    <cfRule type="duplicateValues" dxfId="93" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="duplicateValues" dxfId="92" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="duplicateValues" dxfId="91" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51:B53">
-    <cfRule type="duplicateValues" dxfId="90" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
-    <cfRule type="duplicateValues" dxfId="89" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:A55 A2:A31 A34:A50">
-    <cfRule type="duplicateValues" dxfId="88" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="duplicateValues" dxfId="87" priority="6"/>
+  <conditionalFormatting sqref="B33:B49 B1:B31 B55:B1048576">
+    <cfRule type="duplicateValues" dxfId="90" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="86" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="85" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50:B52">
+    <cfRule type="duplicateValues" dxfId="87" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="duplicateValues" dxfId="86" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
+    <cfRule type="duplicateValues" dxfId="85" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="duplicateValues" dxfId="84" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
     <cfRule type="duplicateValues" dxfId="83" priority="2"/>
@@ -6889,81 +6810,81 @@
     <hyperlink ref="M29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
     <hyperlink ref="K29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
     <hyperlink ref="O29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G33" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G32" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H32" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L32" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="P32" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch"/>
     <hyperlink ref="H33" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L33" location="'Login_magento++'!A1" display="Login_magento"/>
     <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
     <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="K33" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="O33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="P33" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G35" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G38" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H38" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H34" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="I34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J34" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="K34" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="L34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="M34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="N34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
-    <hyperlink ref="H35" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
-    <hyperlink ref="J35" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K35" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="L35" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="M35" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="N35" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="O35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="M36" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="K33" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="L33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="M33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="N33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="J34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K34" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="M35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
     <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
-    <hyperlink ref="H49" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
     <hyperlink ref="I48" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
-    <hyperlink ref="I49" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
+    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
     <hyperlink ref="J48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
-    <hyperlink ref="J49" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login"/>
     <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G49" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G50" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID"/>
-    <hyperlink ref="G41" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="M41" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G42:G43" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="M41:M43" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="H55" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="M48" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N48" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter"/>
-    <hyperlink ref="O48" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification"/>
-    <hyperlink ref="N33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="L49" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="G49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID"/>
+    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="M40" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="M40:M42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="H54" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter"/>
+    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification"/>
+    <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
     <hyperlink ref="L48" location="'EnterContact++'!A1" display="EnterContact"/>
-    <hyperlink ref="K49" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact"/>
     <hyperlink ref="K48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
-    <hyperlink ref="G40" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
     <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G54:G55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
-    <hyperlink ref="H54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="I55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="I54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="J55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="G36" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
-    <hyperlink ref="H36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="I36" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="J36" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="K36" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="L36" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="G37" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
-    <hyperlink ref="I37" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="J37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K38" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="I38" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
-    <hyperlink ref="K37" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="L38" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G53:G54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="J54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="G35" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="H35" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="I35" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="J35" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K35" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L35" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="G36" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="I36" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="J36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="I37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="K36" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L37" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport"/>
     <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport"/>
-    <hyperlink ref="H40" location="'giftCardReport++'!A1" display="giftCardReport"/>
-    <hyperlink ref="G51" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
-    <hyperlink ref="G51:G53" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="G50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="G50:G52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
     <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento"/>
     <hyperlink ref="K2" location="'SapCustomer++'!A1" display="SapCustomer"/>
     <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation"/>
@@ -6981,63 +6902,59 @@
     <hyperlink ref="J17:J21" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
     <hyperlink ref="I2" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
     <hyperlink ref="I3:I6" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="J55" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="G55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="K55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart"/>
     <hyperlink ref="J56" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="I56" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="G56" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
-    <hyperlink ref="H56" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="K56" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart"/>
     <hyperlink ref="J57" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="J58" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="K58" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="G59" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="K57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H59" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart"/>
     <hyperlink ref="H60" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H59" location="'ClearCart++'!A1" display="ClearCart"/>
-    <hyperlink ref="H61" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G60:G61" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="G59:G60" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="G61" location="'ProductSearch++'!A1" display="ProductSearch"/>
     <hyperlink ref="G62" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G63" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G69" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J71" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="K71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail"/>
+    <hyperlink ref="L71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification"/>
+    <hyperlink ref="G56:G57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H56:H57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I56:I57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="G63" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
+    <hyperlink ref="G64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
     <hyperlink ref="G70" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="J72" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G72" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
-    <hyperlink ref="H72" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="I72" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="K72" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail"/>
-    <hyperlink ref="L72" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification"/>
-    <hyperlink ref="G57:G58" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
-    <hyperlink ref="H57:H58" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="I57:I58" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="G64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
-    <hyperlink ref="G65" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
-    <hyperlink ref="G71" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G32" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="H32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="I32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="K32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="H41" location="'ClearCart++'!A1" display="ClearCart++"/>
-    <hyperlink ref="I41" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="I42:I43" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H42:H43" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="H40" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="I40" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I41:I42" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H41:H42" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
     <hyperlink ref="K42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K43" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J43" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="J41:J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L43" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="L41:L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M42" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="J40:J41" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L40:L41" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M41" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
     <hyperlink ref="N42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="N41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="N43" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="O43" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="O41:O42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O40:O41" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="Q41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="Q40" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
     <hyperlink ref="Q42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="Q41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="Q43" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="R41" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="R42:R43" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="R40" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="R41:R42" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="S41" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="S40" location="'SapCustomer++'!A1" display="SapCustomer"/>
     <hyperlink ref="S42" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="S41" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="S43" location="'SapCustomer++'!A1" display="SapCustomer"/>
     <hyperlink ref="J31" location="'ic_CashDepositPayment++'!A1" display="ic_CashDepositPayment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8106,7 +8023,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="97" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>92</v>
@@ -8156,7 +8073,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="97" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>92</v>
@@ -9836,7 +9753,7 @@
         <v>54</v>
       </c>
       <c r="B4" s="67" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C4" s="85" t="s">
         <v>87</v>
@@ -9847,7 +9764,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="67" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C5" s="85" t="s">
         <v>87</v>
@@ -9858,7 +9775,7 @@
         <v>56</v>
       </c>
       <c r="B6" s="67" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C6" s="85" t="s">
         <v>87</v>
@@ -9869,7 +9786,7 @@
         <v>70</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C7" s="85" t="s">
         <v>87</v>
@@ -10666,16 +10583,16 @@
         <v>397</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J2" s="25" t="s">
         <v>76</v>
@@ -10687,16 +10604,16 @@
         <v>73</v>
       </c>
       <c r="M2" s="25" t="s">
+        <v>672</v>
+      </c>
+      <c r="N2" s="25" t="s">
         <v>673</v>
       </c>
-      <c r="N2" s="25" t="s">
-        <v>674</v>
-      </c>
       <c r="O2" s="26" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1">
@@ -10866,13 +10783,13 @@
         <v>397</v>
       </c>
       <c r="F6" s="25" t="s">
+        <v>683</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>684</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="H6" s="25" t="s">
         <v>685</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>686</v>
       </c>
       <c r="I6" s="25" t="s">
         <v>74</v>
@@ -10881,22 +10798,22 @@
         <v>76</v>
       </c>
       <c r="K6" s="25" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>73</v>
       </c>
       <c r="M6" s="25" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="N6" s="25" t="s">
         <v>74</v>
       </c>
       <c r="O6" s="26" t="s">
+        <v>688</v>
+      </c>
+      <c r="P6" s="27" t="s">
         <v>689</v>
-      </c>
-      <c r="P6" s="27" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="4" customFormat="1" ht="30">
@@ -10916,16 +10833,16 @@
         <v>397</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G7" s="25" t="s">
+        <v>654</v>
+      </c>
+      <c r="H7" s="25" t="s">
         <v>655</v>
       </c>
-      <c r="H7" s="25" t="s">
-        <v>656</v>
-      </c>
       <c r="I7" s="25" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>76</v>
@@ -10934,19 +10851,19 @@
         <v>73</v>
       </c>
       <c r="L7" s="25" t="s">
+        <v>652</v>
+      </c>
+      <c r="M7" s="25" t="s">
         <v>653</v>
       </c>
-      <c r="M7" s="25" t="s">
-        <v>654</v>
-      </c>
       <c r="N7" s="25" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="O7" s="26" t="s">
+        <v>657</v>
+      </c>
+      <c r="P7" s="141" t="s">
         <v>658</v>
-      </c>
-      <c r="P7" s="141" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="4" customFormat="1">
@@ -12648,7 +12565,7 @@
         <v>225504</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -12665,7 +12582,7 @@
         <v>225504</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -12682,7 +12599,7 @@
         <v>225504</v>
       </c>
       <c r="E8" s="119" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -12699,7 +12616,7 @@
         <v>225504</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -12767,7 +12684,7 @@
         <v>225504</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -12784,7 +12701,7 @@
         <v>225564</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -12920,7 +12837,7 @@
         <v>225504</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -12988,7 +12905,7 @@
         <v>225504</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -13005,7 +12922,7 @@
         <v>225504</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -13108,7 +13025,7 @@
         <v>225504</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -13125,7 +13042,7 @@
         <v>225504</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -13413,7 +13330,7 @@
         <v>54</v>
       </c>
       <c r="B4" s="67" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C4" s="80" t="s">
         <v>87</v>
@@ -13427,7 +13344,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="67" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C5" s="80" t="s">
         <v>87</v>
@@ -13441,7 +13358,7 @@
         <v>56</v>
       </c>
       <c r="B6" s="67" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C6" s="80">
         <v>1</v>
@@ -13455,7 +13372,7 @@
         <v>56</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C7" s="80">
         <v>2</v>
@@ -13469,7 +13386,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="67" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C8" s="80">
         <v>1</v>
@@ -13553,7 +13470,7 @@
         <v>571</v>
       </c>
       <c r="K1" s="150" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -13570,7 +13487,7 @@
         <v>147</v>
       </c>
       <c r="E2" s="87" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F2" s="86" t="s">
         <v>402</v>
@@ -13698,7 +13615,7 @@
         <v>147</v>
       </c>
       <c r="E6" s="119" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="F6" s="86" t="s">
         <v>402</v>
@@ -13730,7 +13647,7 @@
         <v>147</v>
       </c>
       <c r="E7" s="87" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F7" s="86" t="s">
         <v>406</v>
@@ -13826,7 +13743,7 @@
         <v>147</v>
       </c>
       <c r="E10" s="86" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F10" s="86" t="s">
         <v>406</v>
@@ -13858,7 +13775,7 @@
         <v>147</v>
       </c>
       <c r="E11" s="117" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F11" s="86" t="s">
         <v>402</v>
@@ -13945,7 +13862,7 @@
         <v>54</v>
       </c>
       <c r="B14" s="67" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C14" s="89" t="s">
         <v>87</v>
@@ -13954,7 +13871,7 @@
         <v>147</v>
       </c>
       <c r="E14" s="89" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F14" s="89" t="s">
         <v>406</v>
@@ -13977,7 +13894,7 @@
         <v>55</v>
       </c>
       <c r="B15" s="89" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C15" s="89" t="s">
         <v>87</v>
@@ -13986,7 +13903,7 @@
         <v>147</v>
       </c>
       <c r="E15" s="89" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F15" s="89" t="s">
         <v>406</v>
@@ -13995,7 +13912,7 @@
         <v>407</v>
       </c>
       <c r="H15" s="89" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I15" s="89" t="s">
         <v>310</v>
@@ -14009,7 +13926,7 @@
         <v>56</v>
       </c>
       <c r="B16" s="89" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C16" s="89">
         <v>1</v>
@@ -14018,7 +13935,7 @@
         <v>147</v>
       </c>
       <c r="E16" s="89" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F16" s="89" t="s">
         <v>406</v>
@@ -14041,7 +13958,7 @@
         <v>58</v>
       </c>
       <c r="B17" s="67" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C17" s="89">
         <v>1</v>
@@ -14050,7 +13967,7 @@
         <v>147</v>
       </c>
       <c r="E17" s="89" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F17" s="89" t="s">
         <v>402</v>
@@ -14073,7 +13990,7 @@
         <v>59</v>
       </c>
       <c r="B18" s="67" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C18" s="89">
         <v>1</v>
@@ -14082,7 +13999,7 @@
         <v>147</v>
       </c>
       <c r="E18" s="89" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F18" s="89" t="s">
         <v>402</v>
@@ -14105,7 +14022,7 @@
         <v>60</v>
       </c>
       <c r="B19" s="67" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C19" s="89">
         <v>1</v>
@@ -14114,7 +14031,7 @@
         <v>147</v>
       </c>
       <c r="E19" s="89" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F19" s="89" t="s">
         <v>402</v>
@@ -14137,7 +14054,7 @@
         <v>61</v>
       </c>
       <c r="B20" s="89" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C20" s="89">
         <v>1</v>
@@ -14146,7 +14063,7 @@
         <v>148</v>
       </c>
       <c r="E20" s="74" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F20" s="89" t="s">
         <v>402</v>
@@ -14155,7 +14072,7 @@
         <v>403</v>
       </c>
       <c r="H20" s="89" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I20" s="89">
         <v>6</v>
@@ -14169,7 +14086,7 @@
         <v>68</v>
       </c>
       <c r="B21" s="89" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C21" s="89" t="s">
         <v>87</v>
@@ -14178,13 +14095,13 @@
         <v>147</v>
       </c>
       <c r="E21" s="89" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F21" s="89" t="s">
         <v>406</v>
       </c>
       <c r="G21" s="89" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H21" s="89">
         <v>1</v>
@@ -14201,7 +14118,7 @@
         <v>69</v>
       </c>
       <c r="B22" s="89" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C22" s="89">
         <v>1</v>
@@ -14210,13 +14127,13 @@
         <v>147</v>
       </c>
       <c r="E22" s="89" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F22" s="89" t="s">
         <v>406</v>
       </c>
       <c r="G22" s="89" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H22" s="89" t="s">
         <v>412</v>
@@ -14233,7 +14150,7 @@
         <v>70</v>
       </c>
       <c r="B23" s="67" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C23" s="89" t="s">
         <v>87</v>
@@ -14242,7 +14159,7 @@
         <v>147</v>
       </c>
       <c r="E23" s="89" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F23" s="89" t="s">
         <v>406</v>
@@ -14335,10 +14252,10 @@
         <v>35</v>
       </c>
       <c r="D1" s="93" t="s">
+        <v>602</v>
+      </c>
+      <c r="E1" s="93" t="s">
         <v>603</v>
-      </c>
-      <c r="E1" s="93" t="s">
-        <v>604</v>
       </c>
       <c r="F1" s="93" t="s">
         <v>421</v>
@@ -14349,16 +14266,16 @@
         <v>54</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C2" s="93" t="s">
         <v>87</v>
       </c>
       <c r="D2" s="93" t="s">
+        <v>604</v>
+      </c>
+      <c r="E2" s="92" t="s">
         <v>605</v>
-      </c>
-      <c r="E2" s="92" t="s">
-        <v>606</v>
       </c>
       <c r="F2" s="93">
         <v>11</v>
@@ -14852,10 +14769,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="97" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E12" s="97" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -14869,10 +14786,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="97" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E13" s="97" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -14897,7 +14814,7 @@
         <v>57</v>
       </c>
       <c r="B15" s="67" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C15" s="98">
         <v>1</v>
@@ -14914,7 +14831,7 @@
         <v>64</v>
       </c>
       <c r="B16" s="67" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C16" s="98">
         <v>1</v>
@@ -14931,7 +14848,7 @@
         <v>65</v>
       </c>
       <c r="B17" s="67" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C17" s="98">
         <v>1</v>
@@ -15000,7 +14917,7 @@
         <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -15008,7 +14925,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="106" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C2" s="104">
         <v>1</v>
@@ -15019,7 +14936,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="106" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C3" s="104">
         <v>1</v>
@@ -15030,7 +14947,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C4" s="104">
         <v>1</v>
@@ -15041,7 +14958,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="139" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C5" s="123">
         <v>1</v>
@@ -15121,13 +15038,13 @@
         <v>35</v>
       </c>
       <c r="D1" s="108" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E1" s="108" t="s">
         <v>82</v>
       </c>
       <c r="F1" s="108" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G1" s="108" t="s">
         <v>83</v>
@@ -15147,7 +15064,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="108" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F2" s="108" t="s">
         <v>9</v>
@@ -15176,7 +15093,7 @@
         <v>91</v>
       </c>
       <c r="G3" s="107" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -15216,10 +15133,10 @@
         <v>35</v>
       </c>
       <c r="D1" s="113" t="s">
+        <v>610</v>
+      </c>
+      <c r="E1" s="113" t="s">
         <v>611</v>
-      </c>
-      <c r="E1" s="113" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -15227,7 +15144,7 @@
         <v>70</v>
       </c>
       <c r="B2" s="114" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C2" s="114">
         <v>1</v>
@@ -15294,7 +15211,7 @@
         <v>179</v>
       </c>
       <c r="I1" s="123" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="J1" s="123" t="s">
         <v>173</v>
@@ -15311,7 +15228,7 @@
         <v>70</v>
       </c>
       <c r="B2" s="139" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C2" s="123" t="s">
         <v>87</v>
@@ -15332,7 +15249,7 @@
         <v>299</v>
       </c>
       <c r="I2" s="123" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="J2" s="123" t="s">
         <v>299</v>
@@ -15446,7 +15363,7 @@
         <v>54</v>
       </c>
       <c r="B4" s="67" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C4" s="77" t="s">
         <v>87</v>
@@ -15469,7 +15386,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="67" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C5" s="77" t="s">
         <v>87</v>
@@ -15492,7 +15409,7 @@
         <v>56</v>
       </c>
       <c r="B6" s="67" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C6" s="77" t="s">
         <v>87</v>
@@ -15515,7 +15432,7 @@
         <v>70</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C7" s="77" t="s">
         <v>87</v>
@@ -15816,7 +15733,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -15898,10 +15815,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>126</v>
@@ -15910,7 +15827,7 @@
         <v>128</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="16" t="s">
@@ -15932,10 +15849,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>126</v>
@@ -15944,7 +15861,7 @@
         <v>128</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16" t="s">
@@ -15966,10 +15883,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>126</v>
@@ -15979,7 +15896,7 @@
       </c>
       <c r="H4" s="24"/>
       <c r="I4" s="24" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>127</v>
@@ -16379,7 +16296,7 @@
         <v>66</v>
       </c>
       <c r="K1" s="91" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="L1" s="91" t="s">
         <v>122</v>
@@ -16453,7 +16370,7 @@
         <v>94</v>
       </c>
       <c r="O2" s="122" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="P2" s="117" t="s">
         <v>92</v>
@@ -16482,10 +16399,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="117" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E3" s="117" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F3" s="118" t="s">
         <v>126</v>
@@ -16503,7 +16420,7 @@
         <v>2222224</v>
       </c>
       <c r="K3" s="122" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="L3" s="117" t="s">
         <v>115</v>
@@ -16515,7 +16432,7 @@
         <v>94</v>
       </c>
       <c r="O3" s="122" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="P3" s="117" t="s">
         <v>92</v>
@@ -16606,10 +16523,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="117" t="s">
+        <v>643</v>
+      </c>
+      <c r="E5" s="117" t="s">
         <v>644</v>
-      </c>
-      <c r="E5" s="117" t="s">
-        <v>645</v>
       </c>
       <c r="F5" s="118" t="s">
         <v>126</v>
@@ -16627,7 +16544,7 @@
         <v>2222226</v>
       </c>
       <c r="K5" s="122" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="L5" s="117" t="s">
         <v>115</v>
@@ -16639,7 +16556,7 @@
         <v>94</v>
       </c>
       <c r="O5" s="122" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="P5" s="117" t="s">
         <v>92</v>
@@ -16668,10 +16585,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="117" t="s">
+        <v>645</v>
+      </c>
+      <c r="E6" s="117" t="s">
         <v>646</v>
-      </c>
-      <c r="E6" s="117" t="s">
-        <v>647</v>
       </c>
       <c r="F6" s="118" t="s">
         <v>126</v>
@@ -16689,7 +16606,7 @@
         <v>2222227</v>
       </c>
       <c r="K6" s="122" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="L6" s="117" t="s">
         <v>115</v>
@@ -16701,7 +16618,7 @@
         <v>94</v>
       </c>
       <c r="O6" s="122" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="P6" s="117" t="s">
         <v>92</v>
@@ -16736,7 +16653,7 @@
         <v>95</v>
       </c>
       <c r="F7" s="142" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G7" s="121" t="s">
         <v>116</v>
@@ -16751,7 +16668,7 @@
         <v>2222227</v>
       </c>
       <c r="K7" s="122" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="L7" s="117" t="s">
         <v>115</v>
@@ -18254,7 +18171,7 @@
         <v>35</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -19301,6 +19218,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19449,15 +19375,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
@@ -19467,6 +19384,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19483,21 +19417,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>